<commit_message>
Added - Just like Heaven
</commit_message>
<xml_diff>
--- a/json/movies.xlsx
+++ b/json/movies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="781">
   <si>
     <t>Movie</t>
   </si>
@@ -2349,6 +2349,16 @@
   </si>
   <si>
     <t>TomJerry</t>
+  </si>
+  <si>
+    <t>Just Like Heaven</t>
+  </si>
+  <si>
+    <t>JustLikeHeaven</t>
+  </si>
+  <si>
+    <t>Elizabeth Masterson, an emergency room physician in San Francisco whose work is everything, is in a car crash while on her way to a blind date at her sister's. Three months later, landscape architect David Abbott, needing a fresh start after his wife's death, takes a sublet on Elizabeth's apartment.
+&lt;br&gt; &lt;br&gt;Elizabeth begins to appear in the apartment, and both are confused. She thinks he is a squatter, and he thinks she broke in. They soon realize she moves through walls and objects. Elizabeth does not know who she is, and insists she is not dead. David unsuccessfully tries to have her spirit exorcised. As only David can see and hear her, others think he is hallucinating and talking to himself. Elizabeth asks him to help her discover who she really is.</t>
   </si>
 </sst>
 </file>
@@ -2398,11 +2408,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2709,7 +2722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2719,8 +2732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="G186" sqref="G186"/>
+    <sheetView tabSelected="1" topLeftCell="H172" workbookViewId="0">
+      <selection activeCell="H205" sqref="H205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8038,6 +8051,32 @@
         <v>774</v>
       </c>
     </row>
+    <row r="205" spans="1:8" ht="38.25">
+      <c r="A205" t="s">
+        <v>778</v>
+      </c>
+      <c r="B205" t="s">
+        <v>8</v>
+      </c>
+      <c r="C205" t="s">
+        <v>760</v>
+      </c>
+      <c r="D205">
+        <v>40</v>
+      </c>
+      <c r="E205" s="1">
+        <v>38611</v>
+      </c>
+      <c r="F205" t="s">
+        <v>4</v>
+      </c>
+      <c r="G205" t="s">
+        <v>779</v>
+      </c>
+      <c r="H205" s="4" t="s">
+        <v>780</v>
+      </c>
+    </row>
     <row r="206" spans="1:8">
       <c r="E206" s="3"/>
     </row>

</xml_diff>